<commit_message>
PIN CubeIDE et PCB
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mimib\Documents\1-ENSEA\1 - ESE\Projet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mimib\Documents\1-ENSEA\1 - ESE\Projet\Git\ESE2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F377D0-5808-453B-AF25-A1BC4932A5F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC94DB5E-9740-4A12-B6BD-5D37C9DC313E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{293715AC-6E2F-4FA4-A2F5-890B307E09FB}"/>
   </bookViews>
@@ -544,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD818C14-4CFB-4FDD-80BA-D9DC513E7ABB}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
pcb alim et connecteurs
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mimib\Documents\1-ENSEA\1-ESE\Projet\Git\ESE2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EBB6C8-2A91-48ED-9F56-1EC6BBA07F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E752AF7-271D-4CD0-BDA4-A0B38914D17F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="696" yWindow="696" windowWidth="17280" windowHeight="8964" xr2:uid="{293715AC-6E2F-4FA4-A2F5-890B307E09FB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{293715AC-6E2F-4FA4-A2F5-890B307E09FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -545,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD818C14-4CFB-4FDD-80BA-D9DC513E7ABB}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Ajout lecture courant et enable lidar sur ioc
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mimib\Documents\1-ENSEA\1-ESE\Projet\Git\ESE2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mimib\Documents\1-ENSEA\1-ESE\Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E752AF7-271D-4CD0-BDA4-A0B38914D17F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A57A947-727F-4BF5-9C0C-D96FA4ECFCAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{293715AC-6E2F-4FA4-A2F5-890B307E09FB}"/>
+    <workbookView xWindow="696" yWindow="696" windowWidth="17280" windowHeight="8964" xr2:uid="{293715AC-6E2F-4FA4-A2F5-890B307E09FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Composant</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>Switch</t>
-  </si>
-  <si>
-    <t>Switch alim</t>
   </si>
   <si>
     <t>2 switch par bumper</t>
@@ -121,17 +118,44 @@
 8 pins - Lidar</t>
   </si>
   <si>
-    <t>Pin header coudé</t>
-  </si>
-  <si>
-    <t>4 pins - Module bluetooth</t>
-  </si>
-  <si>
     <t>1 alimentation
 1 détection de contact
 1 détection de bordure
 1 statut (chat ou souris)
 1 erreur</t>
+  </si>
+  <si>
+    <t>Microswitch</t>
+  </si>
+  <si>
+    <t>Bouton poussoir</t>
+  </si>
+  <si>
+    <t>Würth : 472 123 010 111</t>
+  </si>
+  <si>
+    <t>Alim on/off</t>
+  </si>
+  <si>
+    <t>6 pins - Module bluetooth</t>
+  </si>
+  <si>
+    <t>Pin header (Dupont) coudé</t>
+  </si>
+  <si>
+    <t>Farnell : 1668357</t>
+  </si>
+  <si>
+    <t>Diode TVS 3,3V</t>
+  </si>
+  <si>
+    <t>Farnell : 3702487RL</t>
+  </si>
+  <si>
+    <t>Diode TVS 10V</t>
+  </si>
+  <si>
+    <t>Farnell : 3373187RL</t>
   </si>
 </sst>
 </file>
@@ -155,7 +179,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -171,6 +195,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -202,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -219,15 +249,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -543,31 +580,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD818C14-4CFB-4FDD-80BA-D9DC513E7ABB}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5546875" style="1"/>
     <col min="4" max="4" width="24.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="8" t="s">
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>21</v>
       </c>
     </row>
@@ -651,10 +688,10 @@
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="C9" s="4">
         <v>2</v>
@@ -663,10 +700,10 @@
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C10" s="2">
         <v>2</v>
@@ -681,79 +718,117 @@
         <v>16</v>
       </c>
       <c r="C11" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2">
         <v>8</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="4"/>
+        <v>22</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="C13" s="4">
         <v>1</v>
       </c>
-      <c r="D13" s="5"/>
+      <c r="D13" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2">
+        <v>2</v>
+      </c>
+      <c r="D14" s="11"/>
+    </row>
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="2">
-        <v>1</v>
-      </c>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" ht="79.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="C15" s="8">
+        <v>1</v>
+      </c>
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" spans="1:4" ht="79.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4">
-        <v>9</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2">
+        <v>9</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8">
         <v>5</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4">
-        <v>1</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>31</v>
-      </c>
+      <c r="D17" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="12"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>